<commit_message>
Update for new pcb
</commit_message>
<xml_diff>
--- a/Documents/Pinbelegung.xlsx
+++ b/Documents/Pinbelegung.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{230C41A0-C98B-4468-B3A9-21374BD4D4A0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="55">
   <si>
     <t>I2C-Addr</t>
   </si>
@@ -151,12 +152,45 @@
   </si>
   <si>
     <t>X8F18</t>
+  </si>
+  <si>
+    <t>Verfügbare Pins:</t>
+  </si>
+  <si>
+    <t>D4</t>
+  </si>
+  <si>
+    <t>D3</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>D5</t>
+  </si>
+  <si>
+    <t>D6</t>
+  </si>
+  <si>
+    <t>D7</t>
+  </si>
+  <si>
+    <t>D8</t>
+  </si>
+  <si>
+    <t>D9</t>
+  </si>
+  <si>
+    <t>D10</t>
+  </si>
+  <si>
+    <t>D11</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -192,7 +226,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -202,6 +236,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -481,11 +521,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -494,6 +534,7 @@
     <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.140625" customWidth="1"/>
     <col min="5" max="5" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -515,6 +556,9 @@
       <c r="G1" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="I1" s="1" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -529,8 +573,8 @@
       <c r="A3" s="1">
         <v>8</v>
       </c>
-      <c r="B3" s="3">
-        <v>3</v>
+      <c r="B3" s="3" t="s">
+        <v>46</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>19</v>
@@ -547,14 +591,17 @@
       <c r="G3" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="I3" s="5" t="s">
+        <v>45</v>
+      </c>
       <c r="K3" s="4"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>8</v>
       </c>
-      <c r="B4" s="1">
-        <v>4</v>
+      <c r="B4" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>20</v>
@@ -568,13 +615,16 @@
       <c r="F4" t="s">
         <v>36</v>
       </c>
+      <c r="I4" s="6" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>8</v>
       </c>
-      <c r="B5" s="3">
-        <v>5</v>
+      <c r="B5" s="3" t="s">
+        <v>48</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>8</v>
@@ -585,13 +635,16 @@
       <c r="E5">
         <v>4</v>
       </c>
+      <c r="I5" s="5" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>8</v>
       </c>
-      <c r="B6" s="3">
-        <v>6</v>
+      <c r="B6" s="3" t="s">
+        <v>49</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>8</v>
@@ -602,13 +655,16 @@
       <c r="E6">
         <v>3</v>
       </c>
+      <c r="I6" s="5" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>8</v>
       </c>
-      <c r="B7" s="1">
-        <v>8</v>
+      <c r="B7" s="1" t="s">
+        <v>47</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>20</v>
@@ -622,27 +678,33 @@
       <c r="F7" t="s">
         <v>37</v>
       </c>
+      <c r="I7" s="5" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>8</v>
       </c>
-      <c r="B8" s="3">
-        <v>9</v>
+      <c r="B8" s="3" t="s">
+        <v>52</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>10</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
-      <c r="B9" s="3">
-        <v>10</v>
+      <c r="B9" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>8</v>
@@ -653,13 +715,16 @@
       <c r="E9">
         <v>1</v>
       </c>
+      <c r="I9" s="5" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
-      <c r="B10" s="3">
-        <v>11</v>
+      <c r="B10" s="3" t="s">
+        <v>54</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>19</v>
@@ -670,13 +735,16 @@
       <c r="E10">
         <v>-15</v>
       </c>
+      <c r="I10" s="6" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>8</v>
       </c>
-      <c r="B11" s="1">
-        <v>12</v>
+      <c r="B11" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>13</v>
@@ -687,13 +755,16 @@
       <c r="E11">
         <v>4</v>
       </c>
+      <c r="I11" s="6" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>8</v>
       </c>
-      <c r="B12" s="1">
-        <v>13</v>
+      <c r="B12" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>13</v>
@@ -704,13 +775,16 @@
       <c r="E12">
         <v>-4</v>
       </c>
+      <c r="I12" s="5" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>8</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>20</v>
@@ -721,13 +795,16 @@
       <c r="E13">
         <v>15</v>
       </c>
+      <c r="I13" s="5" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>8</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>20</v>
@@ -741,13 +818,16 @@
       <c r="F14" s="1" t="s">
         <v>37</v>
       </c>
+      <c r="I14" s="6" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>8</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>20</v>
@@ -761,13 +841,16 @@
       <c r="F15" s="1" t="s">
         <v>38</v>
       </c>
+      <c r="I15" s="6" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>8</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>5</v>
+        <v>51</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>20</v>
@@ -780,6 +863,9 @@
       </c>
       <c r="F16" s="1" t="s">
         <v>38</v>
+      </c>
+      <c r="I16" s="6" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -794,8 +880,8 @@
       <c r="A18" s="1">
         <v>9</v>
       </c>
-      <c r="B18" s="3">
-        <v>3</v>
+      <c r="B18" s="3" t="s">
+        <v>46</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>8</v>
@@ -808,8 +894,8 @@
       <c r="A19" s="1">
         <v>9</v>
       </c>
-      <c r="B19" s="1">
-        <v>4</v>
+      <c r="B19" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>20</v>
@@ -828,8 +914,8 @@
       <c r="A20" s="1">
         <v>9</v>
       </c>
-      <c r="B20" s="3">
-        <v>5</v>
+      <c r="B20" s="3" t="s">
+        <v>48</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>8</v>
@@ -842,8 +928,8 @@
       <c r="A21" s="1">
         <v>9</v>
       </c>
-      <c r="B21" s="3">
-        <v>6</v>
+      <c r="B21" s="3" t="s">
+        <v>49</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>8</v>
@@ -856,8 +942,8 @@
       <c r="A22" s="1">
         <v>9</v>
       </c>
-      <c r="B22" s="1">
-        <v>8</v>
+      <c r="B22" s="1" t="s">
+        <v>47</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
@@ -866,8 +952,8 @@
       <c r="A23" s="1">
         <v>9</v>
       </c>
-      <c r="B23" s="3">
-        <v>9</v>
+      <c r="B23" s="3" t="s">
+        <v>52</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>8</v>
@@ -886,8 +972,8 @@
       <c r="A24" s="1">
         <v>9</v>
       </c>
-      <c r="B24" s="3">
-        <v>10</v>
+      <c r="B24" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>8</v>
@@ -900,8 +986,8 @@
       <c r="A25" s="1">
         <v>9</v>
       </c>
-      <c r="B25" s="3">
-        <v>11</v>
+      <c r="B25" s="3" t="s">
+        <v>54</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>32</v>
@@ -917,8 +1003,8 @@
       <c r="A26" s="1">
         <v>9</v>
       </c>
-      <c r="B26" s="1">
-        <v>12</v>
+      <c r="B26" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>13</v>
@@ -934,8 +1020,8 @@
       <c r="A27" s="1">
         <v>9</v>
       </c>
-      <c r="B27" s="1">
-        <v>13</v>
+      <c r="B27" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>13</v>
@@ -952,7 +1038,7 @@
         <v>9</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="1" t="s">
@@ -967,7 +1053,7 @@
         <v>9</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>20</v>
@@ -984,7 +1070,7 @@
         <v>9</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="C30" s="1"/>
       <c r="D30" s="1" t="s">
@@ -999,7 +1085,7 @@
         <v>9</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>5</v>
+        <v>51</v>
       </c>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
@@ -1016,8 +1102,8 @@
       <c r="A33" s="1">
         <v>10</v>
       </c>
-      <c r="B33" s="3">
-        <v>3</v>
+      <c r="B33" s="3" t="s">
+        <v>46</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>8</v>
@@ -1033,8 +1119,8 @@
       <c r="A34" s="1">
         <v>10</v>
       </c>
-      <c r="B34" s="1">
-        <v>4</v>
+      <c r="B34" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>20</v>
@@ -1047,8 +1133,8 @@
       <c r="A35" s="1">
         <v>10</v>
       </c>
-      <c r="B35" s="3">
-        <v>5</v>
+      <c r="B35" s="3" t="s">
+        <v>48</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>8</v>
@@ -1064,8 +1150,8 @@
       <c r="A36" s="1">
         <v>10</v>
       </c>
-      <c r="B36" s="3">
-        <v>6</v>
+      <c r="B36" s="3" t="s">
+        <v>49</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>8</v>
@@ -1081,8 +1167,8 @@
       <c r="A37" s="1">
         <v>10</v>
       </c>
-      <c r="B37" s="1">
-        <v>8</v>
+      <c r="B37" s="1" t="s">
+        <v>47</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>20</v>
@@ -1095,8 +1181,8 @@
       <c r="A38" s="1">
         <v>10</v>
       </c>
-      <c r="B38" s="3">
-        <v>9</v>
+      <c r="B38" s="3" t="s">
+        <v>52</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>8</v>
@@ -1112,8 +1198,8 @@
       <c r="A39" s="1">
         <v>10</v>
       </c>
-      <c r="B39" s="3">
-        <v>10</v>
+      <c r="B39" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>8</v>
@@ -1129,8 +1215,8 @@
       <c r="A40" s="1">
         <v>10</v>
       </c>
-      <c r="B40" s="3">
-        <v>11</v>
+      <c r="B40" s="3" t="s">
+        <v>54</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>8</v>
@@ -1146,8 +1232,8 @@
       <c r="A41" s="1">
         <v>10</v>
       </c>
-      <c r="B41" s="1">
-        <v>12</v>
+      <c r="B41" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>20</v>
@@ -1160,8 +1246,8 @@
       <c r="A42" s="1">
         <v>10</v>
       </c>
-      <c r="B42" s="1">
-        <v>13</v>
+      <c r="B42" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>20</v>
@@ -1175,7 +1261,7 @@
         <v>10</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>20</v>
@@ -1189,7 +1275,7 @@
         <v>10</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>20</v>
@@ -1203,7 +1289,7 @@
         <v>10</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>20</v>
@@ -1217,7 +1303,7 @@
         <v>10</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>5</v>
+        <v>51</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>20</v>
@@ -1238,8 +1324,8 @@
       <c r="A48" s="1">
         <v>11</v>
       </c>
-      <c r="B48" s="3">
-        <v>3</v>
+      <c r="B48" s="3" t="s">
+        <v>46</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>20</v>
@@ -1255,8 +1341,8 @@
       <c r="A49" s="1">
         <v>11</v>
       </c>
-      <c r="B49" s="1">
-        <v>4</v>
+      <c r="B49" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>20</v>
@@ -1272,8 +1358,8 @@
       <c r="A50" s="1">
         <v>11</v>
       </c>
-      <c r="B50" s="3">
-        <v>5</v>
+      <c r="B50" s="3" t="s">
+        <v>48</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>20</v>
@@ -1289,8 +1375,8 @@
       <c r="A51" s="1">
         <v>11</v>
       </c>
-      <c r="B51" s="3">
-        <v>6</v>
+      <c r="B51" s="3" t="s">
+        <v>49</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>20</v>
@@ -1306,8 +1392,8 @@
       <c r="A52" s="1">
         <v>11</v>
       </c>
-      <c r="B52" s="1">
-        <v>8</v>
+      <c r="B52" s="1" t="s">
+        <v>47</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>20</v>
@@ -1323,8 +1409,8 @@
       <c r="A53" s="1">
         <v>11</v>
       </c>
-      <c r="B53" s="3">
-        <v>9</v>
+      <c r="B53" s="3" t="s">
+        <v>52</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>20</v>
@@ -1340,8 +1426,8 @@
       <c r="A54" s="1">
         <v>11</v>
       </c>
-      <c r="B54" s="3">
-        <v>10</v>
+      <c r="B54" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>20</v>
@@ -1357,8 +1443,8 @@
       <c r="A55" s="1">
         <v>11</v>
       </c>
-      <c r="B55" s="3">
-        <v>11</v>
+      <c r="B55" s="3" t="s">
+        <v>54</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>20</v>
@@ -1374,8 +1460,8 @@
       <c r="A56" s="1">
         <v>11</v>
       </c>
-      <c r="B56" s="1">
-        <v>12</v>
+      <c r="B56" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>20</v>
@@ -1388,8 +1474,8 @@
       <c r="A57" s="1">
         <v>11</v>
       </c>
-      <c r="B57" s="1">
-        <v>13</v>
+      <c r="B57" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>20</v>
@@ -1403,7 +1489,7 @@
         <v>11</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>20</v>
@@ -1417,7 +1503,7 @@
         <v>11</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>20</v>
@@ -1431,7 +1517,7 @@
         <v>11</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>20</v>
@@ -1445,7 +1531,7 @@
         <v>11</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>5</v>
+        <v>51</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>20</v>

</xml_diff>